<commit_message>
Adding further documentation stuff
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE4E60B-67E7-4691-A799-67FCF32A92E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71318453-749F-4642-B683-8270DADDDE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -891,71 +891,71 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,22 +1259,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59"/>
-      <c r="I1" s="45" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="64"/>
+      <c r="I1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="47"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1315,7 +1315,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="53" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -1341,17 +1341,17 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="47" t="s">
         <v>89</v>
       </c>
       <c r="F4" s="17"/>
@@ -1367,7 +1367,7 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="20" t="s">
         <v>38</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="20" t="s">
         <v>13</v>
       </c>
@@ -1439,10 +1439,10 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="65" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="28" t="s">
@@ -1465,8 +1465,8 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
-      <c r="B9" s="61"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
         <v>28</v>
       </c>
@@ -1487,8 +1487,8 @@
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
-      <c r="B10" s="61"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
@@ -1511,8 +1511,8 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
         <v>30</v>
       </c>
@@ -1533,8 +1533,8 @@
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
@@ -1557,8 +1557,8 @@
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
         <v>35</v>
       </c>
@@ -1579,8 +1579,8 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
-      <c r="I14" s="68" t="s">
+      <c r="I14" s="48" t="s">
         <v>90</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -1602,13 +1602,13 @@
       <c r="L14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M14" s="69">
+      <c r="M14" s="49">
         <v>45271</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="61"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
         <v>32</v>
       </c>
@@ -1620,8 +1620,8 @@
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
         <v>33</v>
       </c>
@@ -1633,8 +1633,8 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="37" t="s">
         <v>34</v>
       </c>
@@ -1646,7 +1646,7 @@
       <c r="G17" s="39"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="60" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1663,24 +1663,24 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="56"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="66" t="s">
+      <c r="D19" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="47" t="s">
         <v>89</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="14" t="s">
         <v>3</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="20" t="s">
         <v>38</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="23" t="s">
         <v>13</v>
       </c>
@@ -1725,10 +1725,10 @@
       <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="56" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="32" t="s">
@@ -1742,8 +1742,8 @@
       <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="28" t="s">
         <v>42</v>
       </c>
@@ -1755,8 +1755,8 @@
       <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="52"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="9" t="s">
         <v>41</v>
       </c>
@@ -1768,8 +1768,8 @@
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="52"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="9" t="s">
         <v>43</v>
       </c>
@@ -1781,8 +1781,8 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="52"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="9" t="s">
         <v>44</v>
       </c>
@@ -1794,8 +1794,8 @@
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="52"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="9" t="s">
         <v>45</v>
       </c>
@@ -1807,8 +1807,8 @@
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="34" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Adding abbreviations to test document registry
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71318453-749F-4642-B683-8270DADDDE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F0FB7-1B6D-4FAE-A5BF-DCD76D2DA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="155">
   <si>
     <t>Pressure proof tests</t>
   </si>
@@ -194,72 +194,9 @@
     <t>TWR2-PRP-06-M-MC-IGN</t>
   </si>
   <si>
-    <t>TWR2-PRP-07-AC-TT-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-08-AC-TR-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-09-BC-TT-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-10-BC-TR-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-12-SIT-TT-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-13-MIT-IC-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-11-SIT-IC-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-14-MIT-TT-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-15-MIT-TR-IGN</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-16-LT-TT-VV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-17-LT-TT-T</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-18-LT-TT-CC</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-19-LT-TT-PA</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-20-LT-TT-PS</t>
-  </si>
-  <si>
     <t>Igniter manufacturing safety rules</t>
   </si>
   <si>
-    <t>TWR2-PRP-21-G-IC-MV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-22-LT-TT-MV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-23-PPT-TC-MV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-24-DO-TT-MV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-25-DC-TT-MV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-26-DOC-TT-MV</t>
-  </si>
-  <si>
-    <t>TWR2-PRP-26-DPO-TT-MV</t>
-  </si>
-  <si>
     <t>TWR2-PRP-97-G-IP-PS</t>
   </si>
   <si>
@@ -309,18 +246,278 @@
   </si>
   <si>
     <t>TWR2-PRP-88-M-MD-T</t>
+  </si>
+  <si>
+    <t>Igniter elaboration checklist</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-07-G-IC-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-08-AC-TT-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-09-AC-TR-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-10-BC-TT-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-11-BC-TR-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-12-SIT-IC-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-13-SIT-TT-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-14-MIT-IC-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-15-MIT-TT-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-16-MIT-TR-IGN</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-17-LT-TT-VV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-18-LT-TT-T</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-19-LT-TT-CC</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-20-LT-TT-PA</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-21-LT-TT-PS</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-22-G-IC-MV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-23-LT-TT-MV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-24-PPT-TC-MV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-25-DO-TT-MV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-26-DC-TT-MV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-27-DOC-TT-MV</t>
+  </si>
+  <si>
+    <t>TWR2-PRP-28-DPO-TT-MV</t>
+  </si>
+  <si>
+    <t>Abbreviations</t>
+  </si>
+  <si>
+    <t>PPT</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>VV</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>IGN</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>Test checklist</t>
+  </si>
+  <si>
+    <t>Vent valve</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Testcard</t>
+  </si>
+  <si>
+    <t>Propulsion system</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>Pressure proof test</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>Ballistic chamber test</t>
+  </si>
+  <si>
+    <t>Atmosphere combustion test</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>Static igniter test</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>Mockup igniter test</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>Leakage test</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>DOC</t>
+  </si>
+  <si>
+    <t>DPO</t>
+  </si>
+  <si>
+    <t>Dynamic opening under pressure</t>
+  </si>
+  <si>
+    <t>Dynamic opening+closing test</t>
+  </si>
+  <si>
+    <t>Dynamic closing test</t>
+  </si>
+  <si>
+    <t>Dynamic opening test</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>Hot fire test</t>
+  </si>
+  <si>
+    <t>Cold flow test</t>
+  </si>
+  <si>
+    <t>PYR</t>
+  </si>
+  <si>
+    <t>Pyrotechnics</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Initial tests</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>Functional tests</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Test report</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Safety rules</t>
+  </si>
+  <si>
+    <t>Integration checklist</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Integration procedure</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Test plan</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Manufacturer documentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -375,7 +572,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,8 +585,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -833,129 +1036,165 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1236,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,33 +1489,39 @@
     <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
-      <c r="I1" s="50" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
+      <c r="I1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="52"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="46"/>
+      <c r="O1" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="74"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1298,719 +1543,962 @@
       <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
       <c r="I3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="20" t="s">
+      <c r="O3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48"/>
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="E4" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="14" t="s">
+      <c r="O4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48"/>
+      <c r="B5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="I5" s="6" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="20" t="s">
+      <c r="O5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="15" t="s">
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48"/>
+      <c r="B6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
       <c r="I6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="20" t="s">
+      <c r="O6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="I7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="L7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="70">
+        <v>45272</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="E8" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="64"/>
+      <c r="G8" s="65"/>
       <c r="I8" s="6" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="I9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="O8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
-      <c r="B10" s="66"/>
+      <c r="O9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="62"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="71" t="s">
+        <v>67</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="I10" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="68"/>
-      <c r="B11" s="66"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="62"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>55</v>
+        <v>29</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>74</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="I11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="68"/>
-      <c r="B12" s="66"/>
+      <c r="O11" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>56</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>75</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="I12" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
-      <c r="B13" s="66"/>
+      <c r="O12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>76</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="I13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="68"/>
-      <c r="B14" s="66"/>
+      <c r="O13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="62"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>77</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
-      <c r="I14" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M14" s="49">
-        <v>45271</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="68"/>
-      <c r="B15" s="66"/>
+      <c r="I14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="4"/>
+      <c r="O14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="62"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>78</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="66"/>
+      <c r="I15" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="43">
+        <v>45271</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="62"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>60</v>
+        <v>32</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>79</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="37" t="s">
+      <c r="O16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="62"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="O17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="63"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="60" t="s">
+      <c r="D18" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="35"/>
+      <c r="O18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="61"/>
-      <c r="B19" s="20" t="s">
+      <c r="D19" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="O19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="55"/>
+      <c r="B20" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="47" t="s">
+      <c r="D20" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="O20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="55"/>
+      <c r="B21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="O21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="55"/>
+      <c r="B22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="O22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="55"/>
+      <c r="B23" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+      <c r="O23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="O24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="53"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="36"/>
+      <c r="O25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="53"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="61"/>
-      <c r="B20" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61"/>
-      <c r="B21" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61"/>
-      <c r="B22" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="40"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>71</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="57"/>
+      <c r="O26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="53"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>72</v>
+        <v>43</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="57"/>
+      <c r="O27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="53"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>73</v>
+        <v>44</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="59"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="34" t="s">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="53"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="4"/>
+      <c r="O29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="53"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
+      <c r="D30" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="5"/>
+      <c r="O30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O31" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="P31" s="75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O32" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="P32" s="75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O33" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="P33" s="75" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O34" s="75" t="s">
+        <v>146</v>
+      </c>
+      <c r="P34" s="75" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O35" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="P35" s="75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O36" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="P36" s="75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O37" s="75" t="s">
+        <v>153</v>
+      </c>
+      <c r="P37" s="75" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
+      <c r="A55" s="32"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
+      <c r="A57" s="32"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="35"/>
+      <c r="A58" s="32"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
+      <c r="A59" s="32"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
+      <c r="A60" s="32"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="35"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="35"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="32"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A19:A23"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B8:B17"/>
-    <mergeCell ref="A8:A17"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="A8:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assigning people responsible for tests documentation
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BDE756-DBA3-4DA6-934D-F0D63E708BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE8C92C-B35A-4A12-AB81-40A36B59F29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="162">
   <si>
     <t>Pressure proof tests</t>
   </si>
@@ -498,18 +498,47 @@
   </si>
   <si>
     <t>Manufacturer documentation</t>
+  </si>
+  <si>
+    <t>Michał Tomporowski</t>
+  </si>
+  <si>
+    <t>Bartosz Rylski</t>
+  </si>
+  <si>
+    <t>Michał Banaszak</t>
+  </si>
+  <si>
+    <t>Jakub Tyszkiewicz</t>
+  </si>
+  <si>
+    <t>Mikołaj Salamon</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Alicja Kwitek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -600,7 +629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -958,17 +987,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1078,132 +1096,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1486,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,19 +1570,19 @@
       <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1575,22 +1593,26 @@
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
+      <c r="E3" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
       <c r="I3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="4"/>
       <c r="O3" s="1" t="s">
@@ -1602,27 +1624,29 @@
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
       <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="4"/>
       <c r="O4" s="1" t="s">
@@ -1637,22 +1661,26 @@
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
       <c r="I5" s="6" t="s">
         <v>55</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="4"/>
       <c r="O5" s="1" t="s">
@@ -1664,25 +1692,29 @@
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="59"/>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="E6" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
       <c r="I6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="4"/>
       <c r="O6" s="1" t="s">
@@ -1694,18 +1726,20 @@
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="60"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="52" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
       <c r="I7" s="6" t="s">
         <v>53</v>
       </c>
@@ -1718,7 +1752,7 @@
       <c r="L7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="50">
+      <c r="M7" s="48">
         <v>45272</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -1735,24 +1769,26 @@
       <c r="B8" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="45"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="I8" s="6" t="s">
         <v>58</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="4"/>
       <c r="O8" s="1" t="s">
@@ -1765,20 +1801,26 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="73"/>
       <c r="B9" s="71"/>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="45"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="I9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4"/>
       <c r="O9" s="1" t="s">
@@ -1794,21 +1836,23 @@
       <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="49" t="s">
         <v>67</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="I10" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L10" s="1"/>
       <c r="M10" s="4"/>
     </row>
@@ -1818,24 +1862,26 @@
       <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="75" t="s">
+        <v>67</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="I11" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="4"/>
-      <c r="O11" s="52" t="s">
+      <c r="O11" s="50" t="s">
         <v>95</v>
       </c>
       <c r="P11" s="1" t="s">
@@ -1848,19 +1894,23 @@
       <c r="C12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="75" t="s">
+        <v>155</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="I12" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="4"/>
       <c r="O12" s="1" t="s">
@@ -1876,20 +1926,22 @@
       <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="75" t="s">
+        <v>155</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="I13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="4"/>
@@ -1900,27 +1952,35 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="73"/>
       <c r="B14" s="71"/>
       <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="75" t="s">
+        <v>155</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
-      <c r="I14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="4"/>
+      <c r="I14" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="41">
+        <v>45271</v>
+      </c>
       <c r="O14" s="1" t="s">
         <v>116</v>
       </c>
@@ -1928,33 +1988,20 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="73"/>
       <c r="B15" s="71"/>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="75" t="s">
+        <v>155</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
-      <c r="I15" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M15" s="43">
-        <v>45271</v>
-      </c>
       <c r="O15" s="1" t="s">
         <v>117</v>
       </c>
@@ -1968,10 +2015,12 @@
       <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="75" t="s">
+        <v>156</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
       <c r="O16" s="1" t="s">
@@ -1987,10 +2036,12 @@
       <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="75" t="s">
+        <v>156</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="O17" s="1" t="s">
@@ -2003,15 +2054,17 @@
     <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="74"/>
       <c r="B18" s="71"/>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35"/>
+      <c r="E18" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
       <c r="O18" s="1" t="s">
         <v>124</v>
       </c>
@@ -2029,12 +2082,14 @@
       <c r="C19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
+      <c r="E19" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
       <c r="O19" s="1" t="s">
         <v>126</v>
       </c>
@@ -2044,20 +2099,20 @@
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="66"/>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
       <c r="O20" s="1" t="s">
         <v>127</v>
       </c>
@@ -2073,12 +2128,14 @@
       <c r="C21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
+      <c r="E21" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
       <c r="O21" s="1" t="s">
         <v>128</v>
       </c>
@@ -2088,18 +2145,20 @@
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="66"/>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
+      <c r="E22" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
       <c r="O22" s="1" t="s">
         <v>129</v>
       </c>
@@ -2109,18 +2168,20 @@
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="66"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="E23" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
       <c r="O23" s="1" t="s">
         <v>134</v>
       </c>
@@ -2135,15 +2196,17 @@
       <c r="B24" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
+      <c r="E24" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
       <c r="O24" s="1" t="s">
         <v>135</v>
       </c>
@@ -2154,15 +2217,17 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="64"/>
       <c r="B25" s="62"/>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="36"/>
+      <c r="E25" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="34"/>
       <c r="O25" s="1" t="s">
         <v>138</v>
       </c>
@@ -2176,10 +2241,12 @@
       <c r="C26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="25" t="s">
+        <v>159</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="4"/>
       <c r="O26" s="1" t="s">
@@ -2195,10 +2262,12 @@
       <c r="C27" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="4"/>
       <c r="O27" s="1" t="s">
@@ -2214,10 +2283,12 @@
       <c r="C28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
     </row>
@@ -2227,10 +2298,12 @@
       <c r="C29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="4"/>
       <c r="O29" s="1" t="s">
@@ -2243,13 +2316,15 @@
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="64"/>
       <c r="B30" s="63"/>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="38" t="s">
+        <v>161</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="5"/>
       <c r="O30" s="1" t="s">
@@ -2316,184 +2391,184 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="32"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="32"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="32"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="32"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="32"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="32"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="32"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="32"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="32"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="32"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Commiting new A2HRM simulation files after cold flow test
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE8C92C-B35A-4A12-AB81-40A36B59F29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C057EF3A-C5C4-4A2A-A400-3DB77D080D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>Static igniter testcard</t>
   </si>
   <si>
-    <t>Leakage testcard</t>
-  </si>
-  <si>
     <t>Plug assembly</t>
   </si>
   <si>
@@ -519,18 +516,29 @@
   </si>
   <si>
     <t>Alicja Kwitek</t>
+  </si>
+  <si>
+    <t>Leakage test checklist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1096,132 +1104,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1504,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,26 +1535,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69"/>
-      <c r="I1" s="55" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
+      <c r="I1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
-      <c r="O1" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="P1" s="54"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58"/>
+      <c r="O1" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1570,24 +1578,24 @@
       <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="36" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1596,11 +1604,11 @@
       <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>68</v>
+      <c r="D3" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
@@ -1608,33 +1616,33 @@
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="4"/>
       <c r="O3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>68</v>
+      <c r="D4" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>67</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
@@ -1642,22 +1650,22 @@
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="4"/>
       <c r="O4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="59"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1665,182 +1673,182 @@
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>157</v>
+        <v>48</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>156</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15"/>
       <c r="I5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="4"/>
       <c r="O5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
+      <c r="D6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
       <c r="I6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="4"/>
       <c r="O6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="60"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="51" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>157</v>
+        <v>50</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>156</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
       <c r="I7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="48">
+        <v>66</v>
+      </c>
+      <c r="M7" s="47">
         <v>45272</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="D8" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="I8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="4"/>
       <c r="O8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="73"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="42" t="s">
+      <c r="A9" s="74"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="E9" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
       <c r="I9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="4"/>
       <c r="O9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="73"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>67</v>
+      <c r="D10" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>66</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
@@ -1848,25 +1856,25 @@
         <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="73"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="75" t="s">
-        <v>67</v>
+      <c r="D11" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>66</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
@@ -1874,31 +1882,31 @@
         <v>18</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="4"/>
-      <c r="O11" s="50" t="s">
-        <v>95</v>
+      <c r="O11" s="49" t="s">
+        <v>94</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="73"/>
-      <c r="B12" s="71"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="75" t="s">
-        <v>155</v>
+      <c r="D12" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>154</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
@@ -1906,31 +1914,31 @@
         <v>24</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="4"/>
       <c r="O12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="73"/>
-      <c r="B13" s="71"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="75" t="s">
-        <v>155</v>
+      <c r="D13" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>154</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
@@ -1938,405 +1946,405 @@
         <v>25</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="4"/>
       <c r="O13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="73"/>
-      <c r="B14" s="71"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="75" t="s">
-        <v>155</v>
+      <c r="D14" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>154</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
-      <c r="I14" s="40" t="s">
+      <c r="I14" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="41">
+        <v>66</v>
+      </c>
+      <c r="M14" s="40">
         <v>45271</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="73"/>
-      <c r="B15" s="71"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="75" t="s">
-        <v>155</v>
+      <c r="D15" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>154</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
       <c r="O15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="73"/>
-      <c r="B16" s="71"/>
+      <c r="A16" s="74"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="75" t="s">
-        <v>156</v>
+      <c r="D16" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>155</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
       <c r="O16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="73"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="75" t="s">
-        <v>156</v>
+      <c r="D17" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>155</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="O17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="P17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="75"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32"/>
+      <c r="O18" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="74"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="66" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="76" t="s">
-        <v>68</v>
+      <c r="C19" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="15"/>
       <c r="O19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="66"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>68</v>
+      <c r="C20" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>67</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="15"/>
       <c r="O20" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="66"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="76" t="s">
-        <v>158</v>
+      <c r="C21" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>157</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="15"/>
       <c r="O21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="66"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="76" t="s">
-        <v>158</v>
+      <c r="C22" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>157</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="15"/>
       <c r="O22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="66"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="46" t="s">
+      <c r="C23" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="O23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="76" t="s">
+      <c r="E24" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+      <c r="O24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="65"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="O23" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P23" s="1" t="s">
+      <c r="F25" s="24"/>
+      <c r="G25" s="33"/>
+      <c r="O25" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="P25" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="65"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
-      <c r="O24" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="25" t="s">
+      <c r="D26" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="34"/>
-      <c r="O25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>159</v>
+      <c r="E26" s="24" t="s">
+        <v>158</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="4"/>
       <c r="O26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="64"/>
-      <c r="B27" s="62"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>161</v>
+        <v>42</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>160</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="4"/>
       <c r="O27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="64"/>
-      <c r="B28" s="62"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>161</v>
+        <v>43</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>160</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
-      <c r="B29" s="62"/>
+      <c r="A29" s="65"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>161</v>
+        <v>44</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>160</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="4"/>
       <c r="O29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="64"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>161</v>
+      <c r="A30" s="65"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>160</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="5"/>
       <c r="O30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O31" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>27</v>
@@ -2344,231 +2352,231 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O32" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P34" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P35" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O36" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="P36" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O37" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="P37" s="1" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="29"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="29"/>
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="30"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Adding distance insulation models, modifying combustion chamber length, updating grains drafts, general work on test documentation
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C057EF3A-C5C4-4A2A-A400-3DB77D080D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D79AB9-A2B9-47D1-B910-7B82DD047A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="163">
   <si>
     <t>Pressure proof tests</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>Leakage test checklist</t>
+  </si>
+  <si>
+    <t>Document number</t>
   </si>
 </sst>
 </file>
@@ -1163,6 +1166,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,7 +1233,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1513,7 +1516,7 @@
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,26 +1538,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="70"/>
-      <c r="I1" s="56" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="71"/>
+      <c r="I1" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58"/>
-      <c r="O1" s="54" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="59"/>
+      <c r="O1" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="55"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1567,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>16</v>
+        <v>162</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>8</v>
@@ -1595,7 +1598,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1631,7 +1634,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="60"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
@@ -1665,7 +1668,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="60"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1699,7 +1702,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="60"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
@@ -1733,7 +1736,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="61"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
@@ -1771,10 +1774,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="72" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1807,8 +1810,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="41" t="s">
         <v>70</v>
       </c>
@@ -1839,8 +1842,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
@@ -1865,8 +1868,8 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
@@ -1897,8 +1900,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="74"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="9" t="s">
         <v>30</v>
       </c>
@@ -1929,8 +1932,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="74"/>
-      <c r="B13" s="72"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
@@ -1961,8 +1964,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="74"/>
-      <c r="B14" s="72"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="73"/>
       <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
@@ -1997,8 +2000,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="74"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="73"/>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
@@ -2018,8 +2021,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="74"/>
-      <c r="B16" s="72"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
@@ -2039,8 +2042,8 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="74"/>
-      <c r="B17" s="72"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
@@ -2060,8 +2063,8 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="75"/>
-      <c r="B18" s="72"/>
+      <c r="A18" s="76"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="30" t="s">
         <v>34</v>
       </c>
@@ -2081,13 +2084,13 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="67" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="54" t="s">
         <v>161</v>
       </c>
       <c r="D19" s="44" t="s">
@@ -2106,11 +2109,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="67"/>
+      <c r="A20" s="68"/>
       <c r="B20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="54" t="s">
         <v>161</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -2129,11 +2132,11 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="67"/>
+      <c r="A21" s="68"/>
       <c r="B21" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="76" t="s">
+      <c r="C21" s="54" t="s">
         <v>161</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -2152,11 +2155,11 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="67"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="54" t="s">
         <v>161</v>
       </c>
       <c r="D22" s="44" t="s">
@@ -2175,11 +2178,11 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="67"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="54" t="s">
         <v>161</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -2198,10 +2201,10 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="63" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -2223,8 +2226,8 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="64"/>
       <c r="C25" s="21" t="s">
         <v>41</v>
       </c>
@@ -2244,8 +2247,8 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="64"/>
       <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
@@ -2265,8 +2268,8 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
-      <c r="B27" s="63"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
@@ -2286,8 +2289,8 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
-      <c r="B28" s="63"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="64"/>
       <c r="C28" s="9" t="s">
         <v>43</v>
       </c>
@@ -2301,8 +2304,8 @@
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="B29" s="63"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="64"/>
       <c r="C29" s="9" t="s">
         <v>44</v>
       </c>
@@ -2322,8 +2325,8 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="65"/>
-      <c r="B30" s="64"/>
+      <c r="A30" s="66"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="27" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Adding color scheme for pointing approval status
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D79AB9-A2B9-47D1-B910-7B82DD047A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909EA991-72AA-4320-B5AC-122B800F17EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="166">
   <si>
     <t>Pressure proof tests</t>
   </si>
@@ -522,6 +522,15 @@
   </si>
   <si>
     <t>Document number</t>
+  </si>
+  <si>
+    <t>Ready for approval</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>To be created</t>
   </si>
 </sst>
 </file>
@@ -620,7 +629,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -639,6 +648,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -1103,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1157,7 +1178,6 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1233,6 +1253,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1515,51 +1541,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.44140625" customWidth="1"/>
-    <col min="16" max="16" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
-      <c r="I1" s="57" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
+      <c r="I1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="59"/>
-      <c r="O1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58"/>
+      <c r="O1" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="56"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P1" s="55"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1597,8 +1623,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1610,7 +1636,7 @@
       <c r="D3" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="52" t="s">
         <v>67</v>
       </c>
       <c r="F3" s="14"/>
@@ -1633,15 +1659,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="61"/>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="60"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="81" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="38" t="s">
@@ -1667,8 +1693,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="61"/>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="60"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1704,7 @@
       <c r="D5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="52" t="s">
         <v>156</v>
       </c>
       <c r="F5" s="14"/>
@@ -1701,18 +1727,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="61"/>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="60"/>
       <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="52" t="s">
         <v>156</v>
       </c>
       <c r="F6" s="22"/>
@@ -1735,18 +1761,18 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="61"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="52" t="s">
         <v>156</v>
       </c>
       <c r="F7" s="14"/>
@@ -1754,7 +1780,7 @@
       <c r="I7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="76" t="s">
         <v>55</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1763,7 +1789,7 @@
       <c r="L7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="46">
         <v>45272</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -1773,17 +1799,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="74" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="71" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="80" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="41" t="s">
@@ -1809,13 +1835,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="75"/>
-      <c r="B9" s="73"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="74"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="80" t="s">
         <v>71</v>
       </c>
       <c r="E9" s="41" t="s">
@@ -1841,16 +1867,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="75"/>
-      <c r="B10" s="73"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="74"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="47" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="7"/>
@@ -1858,7 +1884,7 @@
       <c r="I10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="76" t="s">
         <v>62</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1867,16 +1893,16 @@
       <c r="L10" s="1"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="75"/>
-      <c r="B11" s="73"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="74"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="51" t="s">
         <v>66</v>
       </c>
       <c r="F11" s="7"/>
@@ -1892,23 +1918,23 @@
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="4"/>
-      <c r="O11" s="49" t="s">
+      <c r="O11" s="48" t="s">
         <v>94</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
-      <c r="B12" s="73"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="74"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="51" t="s">
         <v>154</v>
       </c>
       <c r="F12" s="7"/>
@@ -1916,7 +1942,7 @@
       <c r="I12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="76" t="s">
         <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -1931,16 +1957,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="75"/>
-      <c r="B13" s="73"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="74"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="51" t="s">
         <v>154</v>
       </c>
       <c r="F13" s="7"/>
@@ -1963,16 +1989,16 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="75"/>
-      <c r="B14" s="73"/>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="74"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="51" t="s">
         <v>154</v>
       </c>
       <c r="F14" s="7"/>
@@ -1999,16 +2025,16 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="75"/>
-      <c r="B15" s="73"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="74"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="51" t="s">
         <v>154</v>
       </c>
       <c r="F15" s="7"/>
@@ -2020,20 +2046,23 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="75"/>
-      <c r="B16" s="73"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="74"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="51" t="s">
         <v>155</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
+      <c r="I16" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="O16" s="1" t="s">
         <v>119</v>
       </c>
@@ -2041,20 +2070,23 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
-      <c r="B17" s="73"/>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="74"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>155</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
+      <c r="I17" s="76" t="s">
+        <v>163</v>
+      </c>
       <c r="O17" s="1" t="s">
         <v>121</v>
       </c>
@@ -2062,20 +2094,23 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76"/>
-      <c r="B18" s="73"/>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="75"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="30" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="51" t="s">
         <v>155</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="32"/>
+      <c r="I18" s="77" t="s">
+        <v>164</v>
+      </c>
       <c r="O18" s="1" t="s">
         <v>123</v>
       </c>
@@ -2083,20 +2118,20 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="67" t="s">
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="53" t="s">
         <v>161</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="52" t="s">
         <v>67</v>
       </c>
       <c r="F19" s="14"/>
@@ -2108,12 +2143,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="68"/>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="67"/>
       <c r="B20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="53" t="s">
         <v>161</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -2131,18 +2166,18 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="68"/>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="67"/>
       <c r="B21" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="53" t="s">
         <v>161</v>
       </c>
       <c r="D21" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="52" t="s">
         <v>157</v>
       </c>
       <c r="F21" s="14"/>
@@ -2154,18 +2189,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="68"/>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="67"/>
       <c r="B22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="53" t="s">
+      <c r="E22" s="52" t="s">
         <v>157</v>
       </c>
       <c r="F22" s="14"/>
@@ -2177,18 +2212,18 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68"/>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="67"/>
       <c r="B23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="D23" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="53" t="s">
+      <c r="E23" s="52" t="s">
         <v>157</v>
       </c>
       <c r="F23" s="19"/>
@@ -2200,17 +2235,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="62" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E24" s="25" t="s">
@@ -2225,9 +2260,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
-      <c r="B25" s="64"/>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="65"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="21" t="s">
         <v>41</v>
       </c>
@@ -2246,9 +2281,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="66"/>
-      <c r="B26" s="64"/>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="65"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
@@ -2267,9 +2302,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
-      <c r="B27" s="64"/>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="65"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
@@ -2288,9 +2323,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="66"/>
-      <c r="B28" s="64"/>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="65"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="9" t="s">
         <v>43</v>
       </c>
@@ -2303,9 +2338,9 @@
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="66"/>
-      <c r="B29" s="64"/>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="65"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="9" t="s">
         <v>44</v>
       </c>
@@ -2324,9 +2359,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="66"/>
-      <c r="B30" s="65"/>
+    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="65"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="27" t="s">
         <v>45</v>
       </c>
@@ -2345,7 +2380,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O31" s="1" t="s">
         <v>102</v>
       </c>
@@ -2353,7 +2388,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O32" s="1" t="s">
         <v>104</v>
       </c>
@@ -2361,7 +2396,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O33" s="1" t="s">
         <v>143</v>
       </c>
@@ -2369,7 +2404,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O34" s="1" t="s">
         <v>145</v>
       </c>
@@ -2377,7 +2412,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O35" s="1" t="s">
         <v>148</v>
       </c>
@@ -2385,7 +2420,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O36" s="1" t="s">
         <v>150</v>
       </c>
@@ -2393,7 +2428,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="O37" s="1" t="s">
         <v>152</v>
       </c>
@@ -2401,7 +2436,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="28"/>
@@ -2410,7 +2445,7 @@
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="28"/>
@@ -2419,7 +2454,7 @@
       <c r="F45" s="28"/>
       <c r="G45" s="28"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="29"/>
       <c r="B46" s="29"/>
       <c r="C46" s="28"/>
@@ -2428,7 +2463,7 @@
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="29"/>
       <c r="B47" s="29"/>
       <c r="C47" s="28"/>
@@ -2437,7 +2472,7 @@
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="29"/>
       <c r="B48" s="29"/>
       <c r="C48" s="28"/>
@@ -2446,7 +2481,7 @@
       <c r="F48" s="28"/>
       <c r="G48" s="28"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="28"/>
@@ -2455,7 +2490,7 @@
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="29"/>
       <c r="B50" s="29"/>
       <c r="C50" s="28"/>
@@ -2464,7 +2499,7 @@
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
       <c r="B51" s="29"/>
       <c r="C51" s="28"/>
@@ -2473,7 +2508,7 @@
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="29"/>
       <c r="B52" s="29"/>
       <c r="C52" s="28"/>
@@ -2482,7 +2517,7 @@
       <c r="F52" s="28"/>
       <c r="G52" s="28"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
       <c r="B53" s="29"/>
       <c r="C53" s="28"/>
@@ -2491,7 +2526,7 @@
       <c r="F53" s="28"/>
       <c r="G53" s="28"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="29"/>
       <c r="B54" s="29"/>
       <c r="C54" s="28"/>
@@ -2500,7 +2535,7 @@
       <c r="F54" s="28"/>
       <c r="G54" s="28"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="29"/>
       <c r="B55" s="29"/>
       <c r="C55" s="28"/>
@@ -2509,7 +2544,7 @@
       <c r="F55" s="28"/>
       <c r="G55" s="28"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="29"/>
       <c r="B56" s="29"/>
       <c r="C56" s="28"/>
@@ -2518,7 +2553,7 @@
       <c r="F56" s="28"/>
       <c r="G56" s="28"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="29"/>
       <c r="B57" s="29"/>
       <c r="C57" s="28"/>
@@ -2527,7 +2562,7 @@
       <c r="F57" s="28"/>
       <c r="G57" s="28"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="29"/>
       <c r="B58" s="29"/>
       <c r="C58" s="28"/>
@@ -2536,7 +2571,7 @@
       <c r="F58" s="28"/>
       <c r="G58" s="28"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="29"/>
       <c r="B59" s="29"/>
       <c r="C59" s="28"/>
@@ -2545,7 +2580,7 @@
       <c r="F59" s="28"/>
       <c r="G59" s="28"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="29"/>
       <c r="B60" s="29"/>
       <c r="C60" s="28"/>
@@ -2554,7 +2589,7 @@
       <c r="F60" s="28"/>
       <c r="G60" s="28"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="29"/>
       <c r="B61" s="29"/>
       <c r="C61" s="28"/>
@@ -2563,7 +2598,7 @@
       <c r="F61" s="28"/>
       <c r="G61" s="28"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
       <c r="B62" s="29"/>
       <c r="C62" s="28"/>
@@ -2572,7 +2607,7 @@
       <c r="F62" s="28"/>
       <c r="G62" s="28"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="29"/>
       <c r="B63" s="29"/>
       <c r="C63" s="28"/>

</xml_diff>

<commit_message>
Updating test documentation registry
</commit_message>
<xml_diff>
--- a/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
+++ b/05-Tests_documentation/04-Propulsion/TWR2-PRP-TD-01_Propulsion_system_test_campaign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\SR\twardowsky2\05-Tests_documentation\04-Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909EA991-72AA-4320-B5AC-122B800F17EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C5FD4D-1334-496E-89D1-C27174560256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -1124,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1187,6 +1187,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1253,12 +1259,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1541,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,26 +1566,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="70"/>
-      <c r="I1" s="56" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="76"/>
+      <c r="I1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58"/>
-      <c r="O1" s="54" t="s">
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
+      <c r="O1" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="55"/>
+      <c r="P1" s="61"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1624,7 +1626,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1633,7 +1635,7 @@
       <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="57" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -1660,14 +1662,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="59" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="38" t="s">
@@ -1694,14 +1696,14 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="82" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="52" t="s">
@@ -1728,14 +1730,14 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="83" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="52" t="s">
@@ -1762,7 +1764,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="61"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
@@ -1780,7 +1782,7 @@
       <c r="I7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="76" t="s">
+      <c r="J7" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1800,16 +1802,16 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="77" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="58" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="41" t="s">
@@ -1836,12 +1838,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="58" t="s">
         <v>71</v>
       </c>
       <c r="E9" s="41" t="s">
@@ -1868,8 +1870,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
@@ -1884,7 +1886,7 @@
       <c r="I10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="76" t="s">
+      <c r="J10" s="54" t="s">
         <v>62</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1894,8 +1896,8 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
@@ -1926,8 +1928,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="9" t="s">
         <v>30</v>
       </c>
@@ -1942,7 +1944,7 @@
       <c r="I12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="54" t="s">
         <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -1958,8 +1960,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="74"/>
-      <c r="B13" s="72"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
@@ -1990,8 +1992,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="74"/>
-      <c r="B14" s="72"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
@@ -2026,8 +2028,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
@@ -2047,8 +2049,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
-      <c r="B16" s="72"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
@@ -2071,8 +2073,8 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="72"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
@@ -2084,7 +2086,7 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
-      <c r="I17" s="76" t="s">
+      <c r="I17" s="54" t="s">
         <v>163</v>
       </c>
       <c r="O17" s="1" t="s">
@@ -2095,8 +2097,8 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="75"/>
-      <c r="B18" s="72"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="30" t="s">
         <v>34</v>
       </c>
@@ -2108,7 +2110,7 @@
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="32"/>
-      <c r="I18" s="77" t="s">
+      <c r="I18" s="55" t="s">
         <v>164</v>
       </c>
       <c r="O18" s="1" t="s">
@@ -2119,7 +2121,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="72" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -2144,7 +2146,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
+      <c r="A20" s="73"/>
       <c r="B20" s="16" t="s">
         <v>2</v>
       </c>
@@ -2167,7 +2169,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="12" t="s">
         <v>3</v>
       </c>
@@ -2190,14 +2192,14 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="D22" s="79" t="s">
+      <c r="D22" s="57" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="52" t="s">
@@ -2213,14 +2215,14 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="78" t="s">
+      <c r="D23" s="56" t="s">
         <v>85</v>
       </c>
       <c r="E23" s="52" t="s">
@@ -2236,10 +2238,10 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="68" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -2261,8 +2263,8 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="69"/>
       <c r="C25" s="21" t="s">
         <v>41</v>
       </c>
@@ -2282,8 +2284,8 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="65"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="69"/>
       <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
@@ -2303,8 +2305,8 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="65"/>
-      <c r="B27" s="63"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="69"/>
       <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
@@ -2324,8 +2326,8 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="65"/>
-      <c r="B28" s="63"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="69"/>
       <c r="C28" s="9" t="s">
         <v>43</v>
       </c>
@@ -2339,8 +2341,8 @@
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
-      <c r="B29" s="63"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="9" t="s">
         <v>44</v>
       </c>
@@ -2360,8 +2362,8 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="B30" s="64"/>
+      <c r="A30" s="71"/>
+      <c r="B30" s="70"/>
       <c r="C30" s="27" t="s">
         <v>45</v>
       </c>

</xml_diff>